<commit_message>
Database SSH Keys change
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-DRGv2-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-DRGv2-template.xlsx
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="1066">
   <si>
     <t>Region</t>
   </si>
@@ -6757,9 +6757,6 @@
   </si>
   <si>
     <t>bmdb</t>
-  </si>
-  <si>
-    <t>ssh-rsa AAAAB3NzaC1yc2EAAAABJQAAAQEAxQXVLKYOfEPNY6/psWxXWNIN23SFRkaHO2vlUQ3b3vv9k5OO5Di5qmzJ+hZoTifYw+4oyYs0vsPgccy8uz7eJTso2gyk4g7eKMEbmQdDbdPb1K8v1EdF11LfjnImepDDGRNgabhjfS4R/FAA0BTj8xAOjnRsBRD2FrYcVyoxvunKce1V5o3CtgqNlcLrSf+PJb++AW/K5BeLFpJMFCJXSC3QuL0ltYVUp/weA7L/yGOGCSJsv8JzaEekXgGHtuGvpibphYBKtk4sqc6AOWcWGT/6kx7Ntvpg+exdkqGQSDz1krcRyZyQpkQTSaq0Xcld1YZ4u8g5gAl/zDs+7ABRVw== rsa-key-20211111</t>
   </si>
   <si>
     <t xml:space="preserve">18.12.0.0 </t>
@@ -11535,7 +11532,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -11546,7 +11543,7 @@
     <row r="1" spans="1:1" ht="15" thickBot="1"/>
     <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1">
       <c r="A2" s="71" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
   </sheetData>
@@ -11678,7 +11675,7 @@
         <v>878</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="F3" s="35" t="s">
         <v>52</v>
@@ -11732,7 +11729,7 @@
         <v>879</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="F4" s="35" t="s">
         <v>52</v>
@@ -11786,7 +11783,7 @@
         <v>880</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="F5" s="40" t="s">
         <v>52</v>
@@ -11837,10 +11834,10 @@
         <v>870</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="F6" s="40" t="s">
         <v>52</v>
@@ -11852,10 +11849,10 @@
         <v>36</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="K6" s="40" t="s">
         <v>23</v>
@@ -23718,7 +23715,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14.5"/>
@@ -23971,7 +23968,7 @@
         <v>91</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="E5" s="107" t="s">
         <v>1007</v>
@@ -24020,7 +24017,7 @@
         <v>1</v>
       </c>
       <c r="U5" s="56" t="s">
-        <v>1009</v>
+        <v>104</v>
       </c>
       <c r="V5" s="40" t="s">
         <v>344</v>
@@ -36260,7 +36257,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -36368,7 +36365,7 @@
         <v>98</v>
       </c>
       <c r="P2" s="112" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="Q2" s="102" t="s">
         <v>444</v>
@@ -36412,7 +36409,7 @@
         <v>432</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>1004</v>
@@ -36427,7 +36424,7 @@
         <v>338</v>
       </c>
       <c r="I4" s="104" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="J4" s="104" t="s">
         <v>437</v>
@@ -43423,7 +43420,7 @@
         <v>349</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>436</v>
@@ -43443,7 +43440,7 @@
       </c>
       <c r="B6" s="40"/>
       <c r="C6" s="40" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="D6" s="40"/>
       <c r="E6" s="40" t="s">
@@ -43460,7 +43457,7 @@
       </c>
       <c r="B7" s="40"/>
       <c r="C7" s="40" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="40" t="s">
@@ -43477,7 +43474,7 @@
       </c>
       <c r="B8" s="40"/>
       <c r="C8" s="40" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D8" s="40"/>
       <c r="E8" s="40" t="s">
@@ -43511,7 +43508,7 @@
       </c>
       <c r="B10" s="40"/>
       <c r="C10" s="40" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D10" s="40"/>
       <c r="E10" s="40" t="s">
@@ -43528,7 +43525,7 @@
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="40" t="s">
@@ -43545,7 +43542,7 @@
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="40" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D12" s="40"/>
       <c r="E12" s="40" t="s">
@@ -43562,7 +43559,7 @@
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D13" s="40"/>
       <c r="E13" s="40"/>
@@ -43577,7 +43574,7 @@
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="40" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
@@ -48782,7 +48779,7 @@
       <c r="C36" s="38"/>
       <c r="D36" s="38"/>
       <c r="E36" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
@@ -48794,7 +48791,7 @@
       <c r="C37" s="38"/>
       <c r="D37" s="38"/>
       <c r="E37" s="1" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
@@ -48806,7 +48803,7 @@
       <c r="C38" s="38"/>
       <c r="D38" s="38"/>
       <c r="E38" s="1" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
@@ -48818,7 +48815,7 @@
       <c r="C39" s="38"/>
       <c r="D39" s="38"/>
       <c r="E39" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
@@ -48830,7 +48827,7 @@
       <c r="C40" s="38"/>
       <c r="D40" s="38"/>
       <c r="E40" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F40" s="38"/>
       <c r="G40" s="38"/>
@@ -48866,7 +48863,7 @@
       <c r="C43" s="38"/>
       <c r="D43" s="38"/>
       <c r="E43" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="F43" s="38"/>
       <c r="G43" s="38"/>
@@ -49382,7 +49379,7 @@
       <c r="C84" s="38"/>
       <c r="D84" s="38"/>
       <c r="E84" s="38" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="F84" s="38"/>
       <c r="G84" s="38"/>
@@ -49394,7 +49391,7 @@
       <c r="C85" s="38"/>
       <c r="D85" s="38"/>
       <c r="E85" s="38" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="F85" s="38"/>
       <c r="G85" s="38"/>
@@ -49406,7 +49403,7 @@
       <c r="C86" s="38"/>
       <c r="D86" s="38"/>
       <c r="E86" s="38" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="F86" s="38"/>
       <c r="G86" s="38"/>
@@ -49642,7 +49639,7 @@
       <c r="C105" s="38"/>
       <c r="D105" s="38"/>
       <c r="E105" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="F105" s="38"/>
       <c r="G105" s="38"/>
@@ -49654,7 +49651,7 @@
       <c r="C106" s="38"/>
       <c r="D106" s="38"/>
       <c r="E106" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F106" s="38"/>
       <c r="G106" s="38"/>
@@ -49666,7 +49663,7 @@
       <c r="C107" s="38"/>
       <c r="D107" s="38"/>
       <c r="E107" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F107" s="38"/>
       <c r="G107" s="38"/>
@@ -49678,7 +49675,7 @@
       <c r="C108" s="38"/>
       <c r="D108" s="38"/>
       <c r="E108" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="F108" s="38"/>
       <c r="G108" s="38"/>
@@ -49690,7 +49687,7 @@
       <c r="C109" s="38"/>
       <c r="D109" s="38"/>
       <c r="E109" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="F109" s="38"/>
       <c r="G109" s="38"/>
@@ -49702,7 +49699,7 @@
       <c r="C110" s="38"/>
       <c r="D110" s="38"/>
       <c r="E110" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="F110" s="38"/>
       <c r="G110" s="38"/>
@@ -49714,7 +49711,7 @@
       <c r="C111" s="38"/>
       <c r="D111" s="38"/>
       <c r="E111" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="F111" s="38"/>
       <c r="G111" s="38"/>
@@ -49726,7 +49723,7 @@
       <c r="C112" s="38"/>
       <c r="D112" s="38"/>
       <c r="E112" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="F112" s="38"/>
       <c r="G112" s="38"/>
@@ -49738,7 +49735,7 @@
       <c r="C113" s="38"/>
       <c r="D113" s="38"/>
       <c r="E113" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F113" s="38"/>
       <c r="G113" s="38"/>
@@ -50150,7 +50147,7 @@
       <c r="C146" s="38"/>
       <c r="D146" s="38"/>
       <c r="E146" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="F146" s="38"/>
       <c r="G146" s="38"/>
@@ -50162,7 +50159,7 @@
       <c r="C147" s="38"/>
       <c r="D147" s="38"/>
       <c r="E147" s="1" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="F147" s="38"/>
       <c r="G147" s="38"/>
@@ -50174,7 +50171,7 @@
       <c r="C148" s="38"/>
       <c r="D148" s="38"/>
       <c r="E148" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="F148" s="38"/>
       <c r="G148" s="38"/>
@@ -50186,7 +50183,7 @@
       <c r="C149" s="38"/>
       <c r="D149" s="38"/>
       <c r="E149" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="F149" s="38"/>
       <c r="G149" s="38"/>
@@ -50198,7 +50195,7 @@
       <c r="C150" s="38"/>
       <c r="D150" s="38"/>
       <c r="E150" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="F150" s="38"/>
       <c r="G150" s="38"/>
@@ -50210,7 +50207,7 @@
       <c r="C151" s="38"/>
       <c r="D151" s="38"/>
       <c r="E151" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="F151" s="38"/>
       <c r="G151" s="38"/>
@@ -50222,7 +50219,7 @@
       <c r="C152" s="38"/>
       <c r="D152" s="38"/>
       <c r="E152" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="F152" s="38"/>
       <c r="G152" s="38"/>
@@ -50258,7 +50255,7 @@
       <c r="C155" s="38"/>
       <c r="D155" s="38"/>
       <c r="E155" s="38" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F155" s="38"/>
       <c r="G155" s="38"/>
@@ -50654,7 +50651,7 @@
       <c r="C186" s="38"/>
       <c r="D186" s="38"/>
       <c r="E186" s="38" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F186" s="38"/>
       <c r="G186" s="38"/>
@@ -50666,7 +50663,7 @@
       <c r="C187" s="38"/>
       <c r="D187" s="38"/>
       <c r="E187" s="38" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F187" s="38"/>
       <c r="G187" s="38"/>
@@ -50678,7 +50675,7 @@
       <c r="C188" s="38"/>
       <c r="D188" s="38"/>
       <c r="E188" s="38" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F188" s="38"/>
       <c r="G188" s="38"/>
@@ -50690,7 +50687,7 @@
       <c r="C189" s="38"/>
       <c r="D189" s="38"/>
       <c r="E189" s="38" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="F189" s="38"/>
       <c r="G189" s="38"/>
@@ -50702,7 +50699,7 @@
       <c r="C190" s="38"/>
       <c r="D190" s="38"/>
       <c r="E190" s="38" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="F190" s="38"/>
       <c r="G190" s="38"/>
@@ -50714,7 +50711,7 @@
       <c r="C191" s="38"/>
       <c r="D191" s="38"/>
       <c r="E191" s="38" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F191" s="38"/>
       <c r="G191" s="38"/>
@@ -50786,7 +50783,7 @@
       <c r="C197" s="76"/>
       <c r="D197" s="76"/>
       <c r="E197" s="76" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="F197" s="76"/>
       <c r="G197" s="76"/>
@@ -50794,7 +50791,7 @@
     </row>
     <row r="198" spans="1:8" s="40" customFormat="1" ht="29">
       <c r="E198" s="38" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
   </sheetData>
@@ -51440,7 +51437,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="39" customFormat="1" ht="187.75" customHeight="1">
       <c r="A1" s="115" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -51467,7 +51464,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
updated CD3 templates to remove external link prompt
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-DRGv2-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-DRGv2-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop\oci_tools\cd3_automation_toolkit\example\"/>
@@ -11532,7 +11532,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>

</xml_diff>